<commit_message>
Complete Using Open Browswer to merge confli
</commit_message>
<xml_diff>
--- a/CellPhone Numbers.xlsx
+++ b/CellPhone Numbers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -41,42 +41,6 @@
     <t>Emily Smith</t>
   </si>
   <si>
-    <t>David Brown</t>
-  </si>
-  <si>
-    <t>Olivia Martinez</t>
-  </si>
-  <si>
-    <t>Christopher Taylor</t>
-  </si>
-  <si>
-    <t>Sophia Anderson</t>
-  </si>
-  <si>
-    <t>Daniel Thompson</t>
-  </si>
-  <si>
-    <t>Ava Garcia</t>
-  </si>
-  <si>
-    <t>Matthew Rodriguez</t>
-  </si>
-  <si>
-    <t>Isabella Clark</t>
-  </si>
-  <si>
-    <t>James Wilson</t>
-  </si>
-  <si>
-    <t>Charlotte Thomas</t>
-  </si>
-  <si>
-    <t>Alexander White</t>
-  </si>
-  <si>
-    <t>Mia Davis</t>
-  </si>
-  <si>
     <t>0821234567</t>
   </si>
   <si>
@@ -84,24 +48,6 @@
   </si>
   <si>
     <t>0793456789</t>
-  </si>
-  <si>
-    <t>0834567890</t>
-  </si>
-  <si>
-    <t>0645678901</t>
-  </si>
-  <si>
-    <t>0606789012</t>
-  </si>
-  <si>
-    <t>0767890123</t>
-  </si>
-  <si>
-    <t>0748901234</t>
-  </si>
-  <si>
-    <t>0819012345</t>
   </si>
 </sst>
 </file>
@@ -445,7 +391,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +413,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -475,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -483,104 +429,44 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bug Fix And Replace File
</commit_message>
<xml_diff>
--- a/CellPhone Numbers.xlsx
+++ b/CellPhone Numbers.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -41,6 +41,42 @@
     <t>Emily Smith</t>
   </si>
   <si>
+    <t>David Brown</t>
+  </si>
+  <si>
+    <t>Olivia Martinez</t>
+  </si>
+  <si>
+    <t>Christopher Taylor</t>
+  </si>
+  <si>
+    <t>Sophia Anderson</t>
+  </si>
+  <si>
+    <t>Daniel Thompson</t>
+  </si>
+  <si>
+    <t>Ava Garcia</t>
+  </si>
+  <si>
+    <t>Matthew Rodriguez</t>
+  </si>
+  <si>
+    <t>Isabella Clark</t>
+  </si>
+  <si>
+    <t>James Wilson</t>
+  </si>
+  <si>
+    <t>Charlotte Thomas</t>
+  </si>
+  <si>
+    <t>Alexander White</t>
+  </si>
+  <si>
+    <t>Mia Davis</t>
+  </si>
+  <si>
     <t>0821234567</t>
   </si>
   <si>
@@ -48,6 +84,24 @@
   </si>
   <si>
     <t>0793456789</t>
+  </si>
+  <si>
+    <t>0834567890</t>
+  </si>
+  <si>
+    <t>0645678901</t>
+  </si>
+  <si>
+    <t>0606789012</t>
+  </si>
+  <si>
+    <t>0767890123</t>
+  </si>
+  <si>
+    <t>0748901234</t>
+  </si>
+  <si>
+    <t>0819012345</t>
   </si>
 </sst>
 </file>
@@ -391,7 +445,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,7 +467,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -421,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -429,44 +483,104 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>